<commit_message>
Create blackbox test cases
Completed and ready for review
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
+++ b/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea97e295ea41d4c6/Documents/GitHub/summer25-sft221-ndd-4/Documents/Testing/TestDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4579103-AD56-459A-8214-3888C1A2F62C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7776" yWindow="3408" windowWidth="13860" windowHeight="8832" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remainingCapacityKg" sheetId="2" r:id="rId1"/>
@@ -319,13 +319,13 @@
     <t>Edge case</t>
   </si>
   <si>
-    <t>Correct col count</t>
-  </si>
-  <si>
     <t>Zero cols map</t>
   </si>
   <si>
     <t>map(25x0)</t>
+  </si>
+  <si>
+    <t>Correct column count</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -426,8 +426,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -435,21 +435,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,100 +745,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -904,100 +892,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1051,100 +1039,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1198,100 +1186,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1345,100 +1333,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4">
         <v>25</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1468,7 +1456,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1492,100 +1480,100 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4">
         <v>25</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="18">
-        <v>30</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="18">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H9" s="6"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1611,6 +1599,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E152465F8480B049A4BD9447EBC49B6A" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27514298402e41c2fc1d863f783970e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d492b804-31ad-42fe-a456-c890c6533ecb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c25d65bcebb2bdc465362360bf72cc4a" ns2:_="">
     <xsd:import namespace="d492b804-31ad-42fe-a456-c890c6533ecb"/>
@@ -1748,35 +1751,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1799,9 +1777,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Complete blackbox test cases
Create test project and run blackbox tests
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
+++ b/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea97e295ea41d4c6/Documents/GitHub/summer25-sft221-ndd-4/Documents/Testing/TestDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4579103-AD56-459A-8214-3888C1A2F62C}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{441B5508-C1F2-41F6-966B-317D7588A3CB}"/>
   <bookViews>
-    <workbookView xWindow="7776" yWindow="3408" windowWidth="13860" windowHeight="8832" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-432" yWindow="2100" windowWidth="13860" windowHeight="8832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remainingCapacityKg" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>Test #</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>Correct column count</t>
+  </si>
+  <si>
+    <t>Automated?</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -367,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -414,11 +429,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -437,6 +472,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,7 +762,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,18 +772,21 @@
     <col min="3" max="3" width="42.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="42" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="14.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -759,6 +803,12 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -767,6 +817,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -784,6 +836,12 @@
       <c r="E4" t="s">
         <v>24</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -801,6 +859,12 @@
       <c r="E5" t="s">
         <v>27</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -818,6 +882,12 @@
       <c r="E6" t="s">
         <v>33</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -834,6 +904,12 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -850,8 +926,10 @@
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -867,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97ED8DAB-37D1-4A10-8AFE-EB27013BD9CD}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,18 +956,21 @@
     <col min="3" max="3" width="48.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="21.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -906,6 +987,12 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -914,6 +1001,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -931,6 +1020,12 @@
       <c r="E4" t="s">
         <v>35</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -948,6 +1043,12 @@
       <c r="E5" t="s">
         <v>38</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -965,6 +1066,12 @@
       <c r="E6" t="s">
         <v>46</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -981,6 +1088,12 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -997,8 +1110,10 @@
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1015,7 +1130,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,13 +1145,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1053,6 +1170,12 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1061,6 +1184,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1078,6 +1203,12 @@
       <c r="E4" t="s">
         <v>50</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1095,6 +1226,12 @@
       <c r="E5" t="s">
         <v>54</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1112,6 +1249,12 @@
       <c r="E6" t="s">
         <v>56</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1128,6 +1271,12 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1144,8 +1293,10 @@
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1162,7 +1313,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,18 +1323,21 @@
     <col min="3" max="3" width="34.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="37.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="20.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1200,6 +1354,12 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1208,6 +1368,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1225,6 +1387,12 @@
       <c r="E4" t="s">
         <v>61</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1242,6 +1410,12 @@
       <c r="E5" t="s">
         <v>64</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1259,6 +1433,12 @@
       <c r="E6" t="s">
         <v>67</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1275,6 +1455,12 @@
       </c>
       <c r="E7" t="s">
         <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1291,8 +1477,10 @@
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="8">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1455,7 +1643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7C51A8-E44D-482F-BB5B-6ED0912168EE}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1599,21 +1787,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E152465F8480B049A4BD9447EBC49B6A" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27514298402e41c2fc1d863f783970e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d492b804-31ad-42fe-a456-c890c6533ecb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c25d65bcebb2bdc465362360bf72cc4a" ns2:_="">
     <xsd:import namespace="d492b804-31ad-42fe-a456-c890c6533ecb"/>
@@ -1751,10 +1924,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1777,19 +1975,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix BB-013 & BB-014
Fixed the bugs for both tests, updated the excel sheet. Everything passes.
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
+++ b/Documents/Testing/TestDocuments/blackbox-testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea97e295ea41d4c6/Documents/GitHub/summer25-sft221-ndd-4/Documents/Testing/TestDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{441B5508-C1F2-41F6-966B-317D7588A3CB}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{AFA805EA-3E91-48A1-B193-95EB6F7E1872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C1D66B6-27EC-426A-A1B3-8494B0C4D136}"/>
   <bookViews>
-    <workbookView xWindow="-432" yWindow="2100" windowWidth="13860" windowHeight="8832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remainingCapacityKg" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="99">
   <si>
     <t>Test #</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
   <si>
     <t>PASS</t>
@@ -464,12 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -477,6 +468,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,47 +775,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -840,7 +837,7 @@
         <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -863,7 +860,7 @@
         <v>97</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -886,7 +883,7 @@
         <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -909,7 +906,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -945,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97ED8DAB-37D1-4A10-8AFE-EB27013BD9CD}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
@@ -962,47 +959,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1024,7 +1021,7 @@
         <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1047,7 +1044,7 @@
         <v>97</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1070,7 +1067,7 @@
         <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1093,7 +1090,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1145,47 +1142,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1207,7 +1204,7 @@
         <v>97</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1230,7 +1227,7 @@
         <v>97</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1253,7 +1250,7 @@
         <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1276,7 +1273,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1312,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86320C61-3145-416D-BBFF-8D26C6A42A26}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,47 +1326,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1437,7 +1434,7 @@
         <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1460,7 +1457,7 @@
         <v>97</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1512,37 +1509,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1659,37 +1656,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1787,6 +1784,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E152465F8480B049A4BD9447EBC49B6A" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27514298402e41c2fc1d863f783970e0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d492b804-31ad-42fe-a456-c890c6533ecb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c25d65bcebb2bdc465362360bf72cc4a" ns2:_="">
     <xsd:import namespace="d492b804-31ad-42fe-a456-c890c6533ecb"/>
@@ -1924,35 +1936,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1975,9 +1962,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BA08FD-D51D-4965-B628-7711FF1FC27F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d492b804-31ad-42fe-a456-c890c6533ecb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>